<commit_message>
Added references to tex document
</commit_message>
<xml_diff>
--- a/results/Results.xlsx
+++ b/results/Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13380" yWindow="460" windowWidth="15420" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="First" sheetId="1" r:id="rId1"/>
@@ -552,11 +552,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2127137904"/>
-        <c:axId val="2137056640"/>
+        <c:axId val="2121466528"/>
+        <c:axId val="2121458512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2127137904"/>
+        <c:axId val="2121466528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -654,7 +654,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2137056640"/>
+        <c:crossAx val="2121458512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -662,7 +662,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2137056640"/>
+        <c:axId val="2121458512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -774,7 +774,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2127137904"/>
+        <c:crossAx val="2121466528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -795,7 +795,7 @@
           <c:x val="0.70306300884364"/>
           <c:y val="0.106593905260703"/>
           <c:w val="0.295453299229316"/>
-          <c:h val="0.217540939501013"/>
+          <c:h val="0.187448417906095"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -818,7 +818,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1278,11 +1278,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2125708688"/>
-        <c:axId val="-2125702736"/>
+        <c:axId val="-2145485568"/>
+        <c:axId val="-2145479616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2125708688"/>
+        <c:axId val="-2145485568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1380,7 +1380,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125702736"/>
+        <c:crossAx val="-2145479616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1388,7 +1388,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2125702736"/>
+        <c:axId val="-2145479616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1500,7 +1500,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125708688"/>
+        <c:crossAx val="-2145485568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1518,10 +1518,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.682557227814877"/>
+          <c:x val="0.710737539148186"/>
           <c:y val="0.0339193828969053"/>
-          <c:w val="0.313849297318848"/>
-          <c:h val="0.217540939501013"/>
+          <c:w val="0.285668910951348"/>
+          <c:h val="0.173559529017206"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1544,7 +1544,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2004,11 +2004,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2125651984"/>
-        <c:axId val="-2125646032"/>
+        <c:axId val="-2145425232"/>
+        <c:axId val="-2145419280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2125651984"/>
+        <c:axId val="-2145425232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2107,7 +2107,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125646032"/>
+        <c:crossAx val="-2145419280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2115,7 +2115,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2125646032"/>
+        <c:axId val="-2145419280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2223,7 +2223,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125651984"/>
+        <c:crossAx val="-2145425232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2241,10 +2241,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.711770677425652"/>
+          <c:x val="0.721835019716738"/>
           <c:y val="0.106593905260703"/>
-          <c:w val="0.286745786425457"/>
-          <c:h val="0.217540939501013"/>
+          <c:w val="0.276681311575183"/>
+          <c:h val="0.171244714202391"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -2267,7 +2267,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2667,11 +2667,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2069039792"/>
-        <c:axId val="-2069693392"/>
+        <c:axId val="-2146011104"/>
+        <c:axId val="-2146017072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2069039792"/>
+        <c:axId val="-2146011104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2769,7 +2769,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2069693392"/>
+        <c:crossAx val="-2146017072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2777,7 +2777,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2069693392"/>
+        <c:axId val="-2146017072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2889,7 +2889,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2069039792"/>
+        <c:crossAx val="-2146011104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2907,10 +2907,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.657752947066588"/>
+          <c:x val="0.712100751898766"/>
           <c:y val="0.106593905260703"/>
-          <c:w val="0.340763278867598"/>
-          <c:h val="0.249359162491052"/>
+          <c:w val="0.286415420898475"/>
+          <c:h val="0.186859142607174"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -2933,7 +2933,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3333,11 +3333,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2077402704"/>
-        <c:axId val="-2115209632"/>
+        <c:axId val="-2146069024"/>
+        <c:axId val="-2146074992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2077402704"/>
+        <c:axId val="-2146069024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3435,7 +3435,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2115209632"/>
+        <c:crossAx val="-2146074992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3443,7 +3443,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115209632"/>
+        <c:axId val="-2146074992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3555,7 +3555,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2077402704"/>
+        <c:crossAx val="-2146069024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3573,10 +3573,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.636759076990376"/>
+          <c:x val="0.693119745901327"/>
           <c:y val="0.106593905260703"/>
-          <c:w val="0.361757254301546"/>
-          <c:h val="0.217540939501013"/>
+          <c:w val="0.305396585390594"/>
+          <c:h val="0.19439286235054"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -3599,7 +3599,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3999,11 +3999,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2067400240"/>
-        <c:axId val="-2071882768"/>
+        <c:axId val="-2146124352"/>
+        <c:axId val="-2146130320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2067400240"/>
+        <c:axId val="-2146124352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4102,7 +4102,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2071882768"/>
+        <c:crossAx val="-2146130320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4110,7 +4110,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2071882768"/>
+        <c:axId val="-2146130320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4218,7 +4218,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2067400240"/>
+        <c:crossAx val="-2146124352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4236,10 +4236,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.691361056430446"/>
-          <c:y val="0.00324198302027888"/>
-          <c:w val="0.302034940944882"/>
-          <c:h val="0.172848282232877"/>
+          <c:x val="0.711489913398506"/>
+          <c:y val="0.0148160906969962"/>
+          <c:w val="0.281906088731662"/>
+          <c:h val="0.128866834354039"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -4262,7 +4262,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4361,11 +4361,6 @@
               <a:rPr lang="en-US"/>
               <a:t>Normalized</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> II</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -4658,11 +4653,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2077917712"/>
-        <c:axId val="-2080441280"/>
+        <c:axId val="2121431712"/>
+        <c:axId val="2121425744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2077917712"/>
+        <c:axId val="2121431712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4760,7 +4755,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080441280"/>
+        <c:crossAx val="2121425744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4768,7 +4763,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2080441280"/>
+        <c:axId val="2121425744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4874,7 +4869,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2077917712"/>
+        <c:crossAx val="2121431712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4894,8 +4889,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.708527922980216"/>
           <c:y val="0.260986065766169"/>
-          <c:w val="0.226145281135633"/>
-          <c:h val="0.238171837353138"/>
+          <c:w val="0.210042222982997"/>
+          <c:h val="0.157153324584427"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4915,7 +4910,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -5016,7 +5011,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Normalized I</a:t>
+              <a:t>Normalized</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5310,11 +5305,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2082382864"/>
-        <c:axId val="-2078841728"/>
+        <c:axId val="2121350256"/>
+        <c:axId val="2121344176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2082382864"/>
+        <c:axId val="2121350256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5399,7 +5394,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -5418,7 +5413,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2078841728"/>
+        <c:crossAx val="2121344176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5426,7 +5421,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2078841728"/>
+        <c:axId val="2121344176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5533,7 +5528,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082382864"/>
+        <c:crossAx val="2121350256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5551,10 +5546,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.643768632694498"/>
+          <c:x val="0.671948977392319"/>
           <c:y val="0.17511367417101"/>
-          <c:w val="0.252457782399842"/>
-          <c:h val="0.265846733946989"/>
+          <c:w val="0.224277422749692"/>
+          <c:h val="0.152420895304754"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -5574,7 +5569,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -9982,9 +9977,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10012,9 +10007,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>530860</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10044,9 +10039,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>94</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:colOff>568960</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10069,16 +10064,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>543560</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10101,16 +10096,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>111760</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10140,9 +10135,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>95</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>264160</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10176,10 +10171,10 @@
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>784860</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10200,16 +10195,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>73660</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10498,7 +10493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -11162,8 +11157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView topLeftCell="E11" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>